<commit_message>
modified demodata excel file
</commit_message>
<xml_diff>
--- a/Demodata.xlsx
+++ b/Demodata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\eclipse-workspace\ExcelDriven\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\downloded\Javamaven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4594283-C685-420D-BB98-DEB7F2385DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305FB894-E67E-41CF-89B3-C2A155CD0E0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{201B527C-DEC4-4783-9D0F-3E77AED74637}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>TestCase</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>Data3</t>
+  </si>
+  <si>
+    <t>Modify profile</t>
+  </si>
+  <si>
+    <t>mmm</t>
+  </si>
+  <si>
+    <t>nnn</t>
+  </si>
+  <si>
+    <t>ooo</t>
   </si>
 </sst>
 </file>
@@ -443,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73907308-1292-4733-B5B1-888B1A4A6B18}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,6 +537,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>